<commit_message>
Climate_Technology:finance network, US_Stock:data format-csv>>xlxs
</commit_message>
<xml_diff>
--- a/Data/energy_investment_status.xlsx
+++ b/Data/energy_investment_status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jodog\PythonDataWorkplace\Project\Public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1676FFB1-6AD1-4687-94D9-F41EA518FB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4246B2D7-81D5-4621-A61C-D70FD48F2B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6696" yWindow="4368" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Country</t>
   </si>
@@ -81,10 +81,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>CO2/GDP(kg/$)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>2012*</t>
   </si>
   <si>
@@ -116,32 +112,63 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>GDPR</t>
+    <t>• MDB's climate finance flow worldwide 2020 | Statista</t>
+  </si>
+  <si>
+    <t>GDP</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>World GDP Growth Rate 1961-2022 | MacroTrends</t>
-  </si>
-  <si>
-    <t>• MDB's climate finance flow worldwide 2020 | Statista</t>
-  </si>
-  <si>
-    <t>climate finance rate of the multilateral development</t>
+    <t>2011*</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>climate finance flow of the multilateral development</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>trillion</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>billion</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>GDP (current US$) | Data (worldbank.org)</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Korea, Rep.</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;₩&quot;* #,##0.00_-;\-&quot;₩&quot;* #,##0.00_-;_-&quot;₩&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="#,##0.000"/>
     <numFmt numFmtId="177" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;₩&quot;* #,##0.00_-;\-&quot;₩&quot;* #,##0.00_-;_-&quot;₩&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="187" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="183" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -212,14 +239,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="181" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -270,7 +297,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma" xfId="5" xr:uid="{88C1BBDB-59B0-48EE-844F-0AD4261C4B92}"/>
@@ -497,45 +533,49 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="16">
+      <c r="F1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="21">
         <v>27</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="18">
         <v>73.67</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="17">
+        <v>14</v>
+      </c>
+      <c r="B3" s="22">
         <v>26.8</v>
       </c>
       <c r="C3" s="20">
@@ -544,11 +584,11 @@
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="17">
+        <v>15</v>
+      </c>
+      <c r="B4" s="22">
         <v>23.8</v>
       </c>
       <c r="C4" s="20">
@@ -557,11 +597,11 @@
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="17">
+        <v>16</v>
+      </c>
+      <c r="B5" s="22">
         <v>28.3</v>
       </c>
       <c r="C5" s="20">
@@ -570,11 +610,11 @@
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="17">
+        <v>17</v>
+      </c>
+      <c r="B6" s="22">
         <v>25.1</v>
       </c>
       <c r="C6" s="20">
@@ -583,11 +623,11 @@
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="17">
+        <v>18</v>
+      </c>
+      <c r="B7" s="22">
         <v>27.4</v>
       </c>
       <c r="C7" s="20">
@@ -596,11 +636,11 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="17">
+        <v>19</v>
+      </c>
+      <c r="B8" s="22">
         <v>35.200000000000003</v>
       </c>
       <c r="C8" s="20">
@@ -609,11 +649,11 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="17">
+        <v>20</v>
+      </c>
+      <c r="B9" s="22">
         <v>43.1</v>
       </c>
       <c r="C9" s="20">
@@ -622,11 +662,11 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="17">
+        <v>21</v>
+      </c>
+      <c r="B10" s="22">
         <v>61.6</v>
       </c>
       <c r="C10" s="20">
@@ -635,8 +675,11 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="21">
         <v>66</v>
       </c>
       <c r="C11" s="20">
@@ -645,39 +688,39 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="15"/>
       <c r="D13" s="17"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
       <c r="D14" s="17"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
       <c r="D15" s="17"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
@@ -734,8 +777,8 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" display="https://www.macrotrends.net/countries/WLD/world/gdp-growth-rate" xr:uid="{1299730D-EF6C-4423-BC88-0A5817D0D7E0}"/>
-    <hyperlink ref="A14" r:id="rId2" display="https://www.statista.com/statistics/591914/climate-finance-flow-of-multilateral-development-bank-worldwide/" xr:uid="{F9BBFFF8-D15E-41E2-B0C7-8CDE7BF8711C}"/>
+    <hyperlink ref="A14" r:id="rId1" display="https://www.statista.com/statistics/591914/climate-finance-flow-of-multilateral-development-bank-worldwide/" xr:uid="{F9BBFFF8-D15E-41E2-B0C7-8CDE7BF8711C}"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://data.worldbank.org/indicator/NY.GDP.MKTP.CD" xr:uid="{337147D8-11AF-465F-B252-119395E75278}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -748,8 +791,8 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -767,9 +810,7 @@
       <c r="D1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -784,10 +825,6 @@
       <c r="D2" s="13">
         <v>14279.937467430953</v>
       </c>
-      <c r="E2">
-        <f>C2/D2</f>
-        <v>0.7470620949378175</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -802,10 +839,6 @@
       <c r="D3" s="13">
         <v>21433.224697000001</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E11" si="0">C3/D3</f>
-        <v>0.21989224984235231</v>
-      </c>
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -820,10 +853,6 @@
       <c r="D4" s="13">
         <v>5148.781948478173</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>0.20024153485558521</v>
-      </c>
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -838,10 +867,6 @@
       <c r="D5" s="13">
         <v>2870.5040967177733</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0.85072165644782094</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -856,10 +881,6 @@
       <c r="D6" s="13">
         <v>1877.8242737207822</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0.24869206694973164</v>
-      </c>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -874,10 +895,6 @@
       <c r="D7" s="13">
         <v>1391.9525103704761</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0.28161880314125581</v>
-      </c>
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -892,10 +909,6 @@
       <c r="D8" s="13">
         <v>2878.6739124144387</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0.11463611719856735</v>
-      </c>
     </row>
     <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -910,10 +923,6 @@
       <c r="D9" s="13">
         <v>2728.8702467058779</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0.10150720809623584</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -928,10 +937,6 @@
       <c r="D10" s="13">
         <v>3888.3267886274448</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0.1656239392953204</v>
-      </c>
     </row>
     <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -946,50 +951,126 @@
       <c r="D11" s="13">
         <v>1269.4339328059139</v>
       </c>
-      <c r="E11">
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="11">
+        <v>1742015045482.313</v>
+      </c>
+      <c r="I13" s="23">
+        <f>H13*10^(-11)</f>
+        <v>17.42015045482313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="11">
+        <v>14279937467430.953</v>
+      </c>
+      <c r="I14" s="23">
+        <f t="shared" ref="I14:I22" si="0">H14*10^(-11)</f>
+        <v>142.79937467430952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="11">
+        <v>323429888934.25677</v>
+      </c>
+      <c r="I15" s="23">
         <f t="shared" si="0"/>
-        <v>0.28122771163907623</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+        <v>3.2342988893425675</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="G16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="11">
+        <v>3888326788627.4448</v>
+      </c>
+      <c r="I16" s="23">
+        <f t="shared" si="0"/>
+        <v>38.883267886274446</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="11">
+        <v>2728870246705.8779</v>
+      </c>
+      <c r="I17" s="23">
+        <f t="shared" si="0"/>
+        <v>27.288702467058776</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="11">
+        <v>2878673912414.439</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" si="0"/>
+        <v>28.786739124144386</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="11">
+        <v>5148781948478.1729</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" si="0"/>
+        <v>51.487819484781724</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1651422932447.7681</v>
+      </c>
+      <c r="I20" s="23">
+        <f t="shared" si="0"/>
+        <v>16.514229324477679</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="11">
+        <v>119870439113.66211</v>
+      </c>
+      <c r="I21" s="23">
+        <f t="shared" si="0"/>
+        <v>1.1987043911366211</v>
+      </c>
+    </row>
+    <row r="22" spans="7:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="11">
+        <v>21433224697000</v>
+      </c>
+      <c r="I22" s="23">
+        <f t="shared" si="0"/>
+        <v>214.33224697</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>